<commit_message>
Changes according to Benedikt Merz e-mail
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_KARMEN_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_KARMEN_INES.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>index</t>
   </si>
@@ -96,12 +96,6 @@
     <t>fsmuges_tag_NCI</t>
   </si>
   <si>
-    <t>KMT_tag</t>
-  </si>
-  <si>
-    <t>KMF_tag</t>
-  </si>
-  <si>
     <t>na_tag_NCI</t>
   </si>
   <si>
@@ -178,6 +172,15 @@
   </si>
   <si>
     <t>Potassium</t>
+  </si>
+  <si>
+    <t>sugars_NCI</t>
+  </si>
+  <si>
+    <t>KMT_tag_NCI</t>
+  </si>
+  <si>
+    <t>KMF_tag_NCI</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -696,10 +699,10 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>7</v>
@@ -707,10 +710,10 @@
     </row>
     <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>7</v>
@@ -718,10 +721,10 @@
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>7</v>
@@ -730,10 +733,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9"/>
       <c r="B9" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>7</v>
@@ -742,10 +745,10 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10"/>
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>7</v>
@@ -757,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>7</v>
@@ -769,7 +772,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>7</v>
@@ -781,7 +784,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>7</v>
@@ -792,7 +795,7 @@
         <v>17</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>7</v>
@@ -804,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>7</v>
@@ -816,7 +819,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>7</v>
@@ -828,7 +831,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>7</v>
@@ -840,7 +843,7 @@
         <v>21</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>7</v>
@@ -852,7 +855,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>7</v>
@@ -860,10 +863,10 @@
     </row>
     <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>7</v>
@@ -872,10 +875,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21"/>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>7</v>
@@ -884,10 +887,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22"/>
       <c r="B22" s="6" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>7</v>
@@ -896,10 +899,10 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23"/>
       <c r="B23" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>7</v>
@@ -908,10 +911,10 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24"/>
       <c r="B24" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>7</v>
@@ -1379,18 +1382,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -1631,6 +1622,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -1640,23 +1643,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1673,4 +1659,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>